<commit_message>
payslip updated till aug 15
</commit_message>
<xml_diff>
--- a/Pay_slip_excel.xlsx
+++ b/Pay_slip_excel.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="12">
   <si>
     <t xml:space="preserve">Pay Slip Number </t>
   </si>
@@ -57,7 +57,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -68,6 +68,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -101,32 +107,32 @@
   </cellStyleXfs>
   <cellXfs count="12">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="14" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -436,7 +442,7 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
@@ -478,7 +484,7 @@
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -504,7 +510,7 @@
         <v>498.45</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
       <c r="A3" s="5">
         <v>2</v>
       </c>
@@ -530,7 +536,7 @@
         <v>499.51</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
       <c r="A4" s="5">
         <v>3</v>
       </c>
@@ -556,7 +562,7 @@
         <v>499.51</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -582,7 +588,7 @@
         <v>498.45</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
       <c r="A6" s="5">
         <v>5</v>
       </c>
@@ -608,7 +614,7 @@
         <v>499.51</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
       <c r="A7" s="5">
         <v>6</v>
       </c>
@@ -634,7 +640,7 @@
         <v>1008.38</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -660,7 +666,7 @@
         <v>999.02</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
       <c r="A9" s="5">
         <v>8</v>
       </c>
@@ -686,7 +692,7 @@
         <v>2016.75</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
       <c r="A10" s="5">
         <v>9</v>
       </c>
@@ -712,7 +718,7 @@
         <v>2028.06</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
       <c r="A11" s="5">
         <v>10</v>
       </c>
@@ -738,7 +744,7 @@
         <v>500</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
       <c r="A12" s="5">
         <v>11</v>
       </c>
@@ -764,7 +770,7 @@
         <v>1151.78</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
       <c r="A13" s="5">
         <v>12</v>
       </c>
@@ -813,6 +819,84 @@
         <v>501.78</v>
       </c>
       <c r="H14" s="7">
+        <v>1151.78</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+      <c r="A15" s="5">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6">
+        <v>45488</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="5">
+        <v>1400</v>
+      </c>
+      <c r="E15" s="7">
+        <v>248.22</v>
+      </c>
+      <c r="F15" s="5">
+        <v>650</v>
+      </c>
+      <c r="G15" s="7">
+        <v>501.78</v>
+      </c>
+      <c r="H15" s="7">
+        <v>1151.78</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="20.25">
+      <c r="A16" s="5">
+        <v>14</v>
+      </c>
+      <c r="B16" s="6">
+        <v>45505</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="5">
+        <v>1400</v>
+      </c>
+      <c r="E16" s="7">
+        <v>248.22</v>
+      </c>
+      <c r="F16" s="5">
+        <v>650</v>
+      </c>
+      <c r="G16" s="7">
+        <v>501.78</v>
+      </c>
+      <c r="H16" s="7">
+        <v>1151.78</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+      <c r="A17" s="5">
+        <v>14</v>
+      </c>
+      <c r="B17" s="6">
+        <v>45519</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="5">
+        <v>1400</v>
+      </c>
+      <c r="E17" s="7">
+        <v>248.22</v>
+      </c>
+      <c r="F17" s="5">
+        <v>650</v>
+      </c>
+      <c r="G17" s="7">
+        <v>501.78</v>
+      </c>
+      <c r="H17" s="7">
         <v>1151.78</v>
       </c>
     </row>

</xml_diff>